<commit_message>
Completed ridership conversions for database.
</commit_message>
<xml_diff>
--- a/ridership/annual/2016.xlsx
+++ b/ridership/annual/2016.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="220">
   <si>
     <t>Weekday</t>
   </si>
@@ -653,6 +653,27 @@
   </si>
   <si>
     <t>24 Jul 2016</t>
+  </si>
+  <si>
+    <t>25 Jul 2016</t>
+  </si>
+  <si>
+    <t>26 Jul 2016</t>
+  </si>
+  <si>
+    <t>27 Jul 2016</t>
+  </si>
+  <si>
+    <t>28 Jul 2016</t>
+  </si>
+  <si>
+    <t>29 Jul 2016</t>
+  </si>
+  <si>
+    <t>30 Jul 2016</t>
+  </si>
+  <si>
+    <t>31 Jul 2016</t>
   </si>
 </sst>
 </file>
@@ -743,9 +764,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$202</c:f>
+              <c:f>Ridership!$B$2:$B$209</c:f>
               <c:strCache>
-                <c:ptCount val="201"/>
+                <c:ptCount val="208"/>
                 <c:pt idx="0">
                   <c:v>02 Jan 2016</c:v>
                 </c:pt>
@@ -1348,16 +1369,37 @@
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>24 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>25 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>26 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>27 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>28 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>29 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>30 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>31 Jul 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$C$2:$C$202</c:f>
+              <c:f>Ridership!$C$2:$C$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="201"/>
+                <c:ptCount val="208"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -1920,7 +1962,7 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>183</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>176</c:v>
@@ -1953,13 +1995,34 @@
                   <c:v>201</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>252</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="199">
                   <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>185</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>209</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1983,9 +2046,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$202</c:f>
+              <c:f>Ridership!$B$2:$B$209</c:f>
               <c:strCache>
-                <c:ptCount val="201"/>
+                <c:ptCount val="208"/>
                 <c:pt idx="0">
                   <c:v>02 Jan 2016</c:v>
                 </c:pt>
@@ -2588,16 +2651,37 @@
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>24 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>25 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>26 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>27 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>28 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>29 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>30 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>31 Jul 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$D$2:$D$202</c:f>
+              <c:f>Ridership!$D$2:$D$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="201"/>
+                <c:ptCount val="208"/>
                 <c:pt idx="0">
                   <c:v>19.13</c:v>
                 </c:pt>
@@ -3160,7 +3244,7 @@
                   <c:v>28.74</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>86.2</c:v>
+                  <c:v>86.53</c:v>
                 </c:pt>
                 <c:pt idx="188">
                   <c:v>87.41</c:v>
@@ -3181,7 +3265,7 @@
                   <c:v>30.09</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>87.78</c:v>
+                  <c:v>88.1</c:v>
                 </c:pt>
                 <c:pt idx="195">
                   <c:v>88.91</c:v>
@@ -3193,13 +3277,34 @@
                   <c:v>94.17</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>89.4</c:v>
+                  <c:v>89.7</c:v>
                 </c:pt>
                 <c:pt idx="199">
                   <c:v>37.86</c:v>
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>31.49</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>90.4</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>91.98</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>98.04</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>95.98</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>92.34</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>39.73</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>32.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3223,9 +3328,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Ridership!$B$2:$B$202</c:f>
+              <c:f>Ridership!$B$2:$B$209</c:f>
               <c:strCache>
-                <c:ptCount val="201"/>
+                <c:ptCount val="208"/>
                 <c:pt idx="0">
                   <c:v>02 Jan 2016</c:v>
                 </c:pt>
@@ -3828,16 +3933,37 @@
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>24 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>25 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>26 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>27 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>28 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>29 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>30 Jul 2016</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>31 Jul 2016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Ridership!$E$2:$E$202</c:f>
+              <c:f>Ridership!$E$2:$E$209</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="201"/>
+                <c:ptCount val="208"/>
                 <c:pt idx="0">
                   <c:v>37.97</c:v>
                 </c:pt>
@@ -4440,6 +4566,27 @@
                 </c:pt>
                 <c:pt idx="200">
                   <c:v>68.51</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>68.66</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>68.81</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>68.96</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>69.11</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>69.26</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>69.41</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>69.56</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4532,13 +4679,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>204</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>218</xdr:row>
+      <xdr:row>225</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4846,7 +4993,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E209"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8063,10 +8210,10 @@
         <v>199</v>
       </c>
       <c r="C189">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="D189">
-        <v>86.2</v>
+        <v>86.53</v>
       </c>
       <c r="E189">
         <v>66.56</v>
@@ -8185,7 +8332,7 @@
         <v>151</v>
       </c>
       <c r="D196">
-        <v>87.78</v>
+        <v>88.1</v>
       </c>
       <c r="E196">
         <v>67.61</v>
@@ -8250,10 +8397,10 @@
         <v>210</v>
       </c>
       <c r="C200">
-        <v>252</v>
+        <v>265</v>
       </c>
       <c r="D200">
-        <v>89.4</v>
+        <v>89.7</v>
       </c>
       <c r="E200">
         <v>68.21</v>
@@ -8291,6 +8438,125 @@
       </c>
       <c r="E202">
         <v>68.51</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" t="s">
+        <v>9</v>
+      </c>
+      <c r="B203" t="s">
+        <v>213</v>
+      </c>
+      <c r="C203">
+        <v>185</v>
+      </c>
+      <c r="D203">
+        <v>90.4</v>
+      </c>
+      <c r="E203">
+        <v>68.66</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" t="s">
+        <v>11</v>
+      </c>
+      <c r="B204" t="s">
+        <v>214</v>
+      </c>
+      <c r="C204">
+        <v>236</v>
+      </c>
+      <c r="D204">
+        <v>91.98</v>
+      </c>
+      <c r="E204">
+        <v>68.81</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" t="s">
+        <v>13</v>
+      </c>
+      <c r="B205" t="s">
+        <v>215</v>
+      </c>
+      <c r="C205">
+        <v>209</v>
+      </c>
+      <c r="D205">
+        <v>98.04</v>
+      </c>
+      <c r="E205">
+        <v>68.96</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" t="s">
+        <v>15</v>
+      </c>
+      <c r="B206" t="s">
+        <v>216</v>
+      </c>
+      <c r="C206">
+        <v>179</v>
+      </c>
+      <c r="D206">
+        <v>95.98</v>
+      </c>
+      <c r="E206">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" t="s">
+        <v>17</v>
+      </c>
+      <c r="B207" t="s">
+        <v>217</v>
+      </c>
+      <c r="C207">
+        <v>206</v>
+      </c>
+      <c r="D207">
+        <v>92.34</v>
+      </c>
+      <c r="E207">
+        <v>69.26</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" t="s">
+        <v>5</v>
+      </c>
+      <c r="B208" t="s">
+        <v>218</v>
+      </c>
+      <c r="C208">
+        <v>122</v>
+      </c>
+      <c r="D208">
+        <v>39.73</v>
+      </c>
+      <c r="E208">
+        <v>69.41</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" t="s">
+        <v>7</v>
+      </c>
+      <c r="B209" t="s">
+        <v>219</v>
+      </c>
+      <c r="C209">
+        <v>100</v>
+      </c>
+      <c r="D209">
+        <v>32.98</v>
+      </c>
+      <c r="E209">
+        <v>69.56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>